<commit_message>
added confound analysis and new data files
</commit_message>
<xml_diff>
--- a/LG_pair_table.xlsx
+++ b/LG_pair_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E39BA2A-8D54-EC4F-B79A-1A86564EE83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07CD580-F1E0-B34F-895D-00B3EE393D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9540" yWindow="500" windowWidth="26840" windowHeight="14980" xr2:uid="{5E5E7DE4-F688-BB48-8D83-B849A4B9DE13}"/>
   </bookViews>
@@ -517,13 +517,16 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>